<commit_message>
Corrige conflictos en server.js
</commit_message>
<xml_diff>
--- a/leads.xlsx
+++ b/leads.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="2025-06-05" sheetId="1" r:id="rId1"/>
     <sheet name="2025-06-04" sheetId="2" r:id="rId2"/>
+    <sheet name="2025-06-06" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -713,4 +714,47 @@
     <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>FECHA</v>
+      </c>
+      <c r="B1" t="str">
+        <v>TEAM</v>
+      </c>
+      <c r="C1" t="str">
+        <v>AGENTE</v>
+      </c>
+      <c r="D1" t="str">
+        <v>NÚMERO</v>
+      </c>
+      <c r="E1" t="str">
+        <v>SERVICIO</v>
+      </c>
+      <c r="F1" t="str">
+        <v>PUNTOS</v>
+      </c>
+      <c r="G1" t="str">
+        <v>CUENTA</v>
+      </c>
+      <c r="H1" t="str">
+        <v>DIRECCIÓN</v>
+      </c>
+      <c r="I1" t="str">
+        <v>ZIP CODE</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Describe brevemente tus      cambios
</commit_message>
<xml_diff>
--- a/leads.xlsx
+++ b/leads.xlsx
@@ -1,47 +1,196 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915"/>
+  </bookViews>
   <sheets>
-    <sheet name="2025-06-07" sheetId="1" r:id="rId1"/>
+    <sheet name="2025-06-08" sheetId="2" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="51">
+  <si>
+    <t>TEAM RANDAL</t>
+  </si>
+  <si>
+    <t>JULIO MEJIA</t>
+  </si>
+  <si>
+    <t>OPTIMO MAS</t>
+  </si>
+  <si>
+    <t>1,00</t>
+  </si>
+  <si>
+    <t>3017 E 149TH AVE, LUTZ, FL 33559</t>
+  </si>
+  <si>
+    <t>FRONTIER 500</t>
+  </si>
+  <si>
+    <t>ANDERSON GUZMAN</t>
+  </si>
+  <si>
+    <t>2307 N Johnson St APT B Plant City FL 33563</t>
+  </si>
+  <si>
+    <t>TEAM ROBERTO</t>
+  </si>
+  <si>
+    <t>FRANCISCO AGUILAR</t>
+  </si>
+  <si>
+    <t>SPECTRUM 1G</t>
+  </si>
+  <si>
+    <t>077 RIVERSIDE DR APT RESNO NV 89503</t>
+  </si>
+  <si>
+    <t>300 MBPS AT&amp;T</t>
+  </si>
+  <si>
+    <t>1,25</t>
+  </si>
+  <si>
+    <t>105 Heflin Ct, San Antonio, TX 78210</t>
+  </si>
+  <si>
+    <t>TEAM IRANIA</t>
+  </si>
+  <si>
+    <t>IRVIN CRUZ</t>
+  </si>
+  <si>
+    <t>809 E Del Mar Ct Compton CA 90221</t>
+  </si>
+  <si>
+    <t>JOHANA SANTANA</t>
+  </si>
+  <si>
+    <t>5605 Squirrel Chase LOTE A16 Ct Youngsville NC 27596</t>
+  </si>
+  <si>
+    <t>YULISSA RUBIO</t>
+  </si>
+  <si>
+    <t>5010 Nispero Ln Laredo TX 78046</t>
+  </si>
+  <si>
+    <t>GISELL DIAZ</t>
+  </si>
+  <si>
+    <t>50 MBPS AT&amp;T</t>
+  </si>
+  <si>
+    <t>0,35</t>
+  </si>
+  <si>
+    <t>1051 Grandview Blvd Kansas City KS 66102</t>
+  </si>
+  <si>
+    <t>PRISCILA HERNANDEZ</t>
+  </si>
+  <si>
+    <t>225 AT&amp;T AIR</t>
+  </si>
+  <si>
+    <t>6600 WISTERIA DR, APT 11, CHARLOTTE, NC 28210</t>
+  </si>
+  <si>
+    <t>1681 GRANITEWAY LN, COLUMBUS, OH 43229</t>
+  </si>
+  <si>
+    <t>1403 E 127th Ave Tampa FL 33612</t>
+  </si>
+  <si>
+    <t>ESTEFANY AMAYA</t>
+  </si>
+  <si>
+    <t>4931 Signature Dr, APT 303 Myrtle Beach SC 29579</t>
+  </si>
+  <si>
+    <t>ROXANA MARTINEZ</t>
+  </si>
+  <si>
+    <t>SPECTRUM 500</t>
+  </si>
+  <si>
+    <t>5421 GOVERNOURS WAY, APT A, LOUISVILLE, KY 40291</t>
+  </si>
+  <si>
+    <t>1270 Sycamore St Greenfield CA 93927</t>
+  </si>
+  <si>
+    <t>JOSUE RENDEROS</t>
+  </si>
+  <si>
+    <t>7710 Lawn Ave Cleveland OH 44102</t>
+  </si>
+  <si>
+    <t>1412 E 140th Ave APT B Tampa FL 33613</t>
+  </si>
+  <si>
+    <t>2920 Chapel Hill Rd Apt 16B, Durham, NC 27707</t>
+  </si>
+  <si>
+    <t>1G AT&amp;T</t>
+  </si>
+  <si>
+    <t>1,50</t>
+  </si>
+  <si>
+    <t>1544 ANTIGUA BAY DR, ORLANDO, FL 32824</t>
+  </si>
+  <si>
+    <t>770 HORIZON PKWY, BUFORD, GA 30518</t>
+  </si>
+  <si>
+    <t>2052 S 35th St Milwaukee WI 53215</t>
+  </si>
+  <si>
+    <t>9005 Kennedy St Riverside CA 92509</t>
+  </si>
+  <si>
+    <t>4811 Belmont Ave Dallas TX 75204</t>
+  </si>
+  <si>
+    <t>SPECTRUM DOUBLE PLAY PREMIER</t>
+  </si>
+  <si>
+    <t>845 1st St SW Birmingham AL 35211</t>
+  </si>
+  <si>
+    <t>ALEXIS</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,7 +201,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -60,18 +209,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,14 +574,661 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
   </sheetViews>
-  <sheetData/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
-  </ignoredErrors>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>8136138533</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>8136138533</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>8636774147</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>7758430944</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>8303268024</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>3239441193</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>9193258491</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>9569994061</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>9133753569</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>7042014006</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>6146033758</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>8134664156</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>9531956755</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>3466079166</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>8316575470</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16">
+        <v>2162987852</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>6787892917</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <v>9195190991</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>4078738245</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>4046712155</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21">
+        <v>4143063825</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>9518368153</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>2149279633</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>2149279633</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>45816</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>2516550998</v>
+      </c>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>